<commit_message>
breaking changes accepts xlsx
</commit_message>
<xml_diff>
--- a/example/bgg.xlsx
+++ b/example/bgg.xlsx
@@ -13,10 +13,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Game Name</t>
+    <t>id</t>
   </si>
   <si>
-    <t>BGG ID</t>
+    <t>name</t>
   </si>
   <si>
     <t>Settlers of Catan</t>

</xml_diff>